<commit_message>
Expanding functionality to retrieve both times and distances
</commit_message>
<xml_diff>
--- a/data/Depot Information Sample.xlsx
+++ b/data/Depot Information Sample.xlsx
@@ -696,7 +696,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -730,6 +730,11 @@
           <t>Driving Time (minutes)</t>
         </is>
       </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>Driving Distance (miles)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -753,7 +758,10 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>17.51666666666667</v>
+        <v>12</v>
+      </c>
+      <c r="F2" t="n">
+        <v>6.6524</v>
       </c>
     </row>
   </sheetData>

</xml_diff>